<commit_message>
Issue #219 change to build Any CPU and refactor Excel and CSV reading code to support
</commit_message>
<xml_diff>
--- a/JosephM.Deployment.Test/Files/AccountsWithKeys.xlsx
+++ b/JosephM.Deployment.Test/Files/AccountsWithKeys.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseph.mcgregor-macd\Desktop\Test Imports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseph.mcgregor-macd\source\repos\XRM-Developer-Tool\JosephM.Deployment.Test\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,9 +26,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
-    <t>Account Number</t>
-  </si>
-  <si>
     <t>Account Name</t>
   </si>
   <si>
@@ -66,6 +63,9 @@
   </si>
   <si>
     <t>Sydeny</t>
+  </si>
+  <si>
+    <t>accountnumber</t>
   </si>
 </sst>
 </file>
@@ -386,76 +386,76 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1234567</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>7654321</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>11223344</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>